<commit_message>
excel sheet data fetch
</commit_message>
<xml_diff>
--- a/resource/Book1.xlsx
+++ b/resource/Book1.xlsx
@@ -96,18 +96,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,18 +122,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="A3" sqref="A3:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +423,9 @@
     <col min="4" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="9.140625" style="1"/>
-    <col min="13" max="15" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -488,40 +480,40 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>26</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>4</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>1991</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>4</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>21</v>
       </c>
       <c r="M2" s="3">
@@ -530,21 +522,12 @@
       <c r="N2" s="3">
         <v>9595507502</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>9595507502</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>